<commit_message>
Fixed some naming issues
</commit_message>
<xml_diff>
--- a/Resources/Lookup Changes.xlsx
+++ b/Resources/Lookup Changes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\connachan.cara\Documents\pop_projections_shiny_tool\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8E8609-447C-47F7-A5D7-022DBEFE9BBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2291F83-95B4-46BC-B43F-8FC9F6DFC842}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{3687BCDE-84BD-47C3-873F-9218EE481B65}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="296">
   <si>
     <t>Airyhal</t>
   </si>
@@ -926,12 +926,6 @@
   </si>
   <si>
     <t>Council Name</t>
-  </si>
-  <si>
-    <t>ArbroEaL</t>
-  </si>
-  <si>
-    <t>ArbroEal</t>
   </si>
 </sst>
 </file>
@@ -5640,10 +5634,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88159FC9-125C-4960-B11E-EF32BCBF7347}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD31"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5862,241 +5856,227 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>40</v>
+      <c r="A15" t="str">
+        <f t="array" ref="A15">INDEX('[1]Lookup Changes'!$C$2:$C$346,MATCH('[1]Short Name errors'!C16,'[1]Lookup Changes'!$A$2:$A$346,0))</f>
+        <v>East Ayrshire</v>
       </c>
       <c r="B15" t="s">
-        <v>296</v>
+        <v>279</v>
       </c>
       <c r="C15" t="s">
-        <v>297</v>
+        <v>61</v>
       </c>
       <c r="D15" t="s">
-        <v>297</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
-        <f t="array" ref="A16">INDEX('[1]Lookup Changes'!$C$2:$C$346,MATCH('[1]Short Name errors'!C16,'[1]Lookup Changes'!$A$2:$A$346,0))</f>
+        <f t="array" ref="A16">INDEX('[1]Lookup Changes'!$C$2:$C$346,MATCH('[1]Short Name errors'!C17,'[1]Lookup Changes'!$A$2:$A$346,0))</f>
         <v>East Ayrshire</v>
       </c>
       <c r="B16" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D16" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
-        <f t="array" ref="A17">INDEX('[1]Lookup Changes'!$C$2:$C$346,MATCH('[1]Short Name errors'!C17,'[1]Lookup Changes'!$A$2:$A$346,0))</f>
+        <f t="array" ref="A17">INDEX('[1]Lookup Changes'!$C$2:$C$346,MATCH('[1]Short Name errors'!C18,'[1]Lookup Changes'!$A$2:$A$346,0))</f>
         <v>East Ayrshire</v>
       </c>
       <c r="B17" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C17" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D17" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
-        <f t="array" ref="A18">INDEX('[1]Lookup Changes'!$C$2:$C$346,MATCH('[1]Short Name errors'!C18,'[1]Lookup Changes'!$A$2:$A$346,0))</f>
+        <f t="array" ref="A18">INDEX('[1]Lookup Changes'!$C$2:$C$346,MATCH('[1]Short Name errors'!C19,'[1]Lookup Changes'!$A$2:$A$346,0))</f>
         <v>East Ayrshire</v>
       </c>
       <c r="B18" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C18" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D18" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
-        <f t="array" ref="A19">INDEX('[1]Lookup Changes'!$C$2:$C$346,MATCH('[1]Short Name errors'!C19,'[1]Lookup Changes'!$A$2:$A$346,0))</f>
+        <f t="array" ref="A19">INDEX('[1]Lookup Changes'!$C$2:$C$346,MATCH('[1]Short Name errors'!C20,'[1]Lookup Changes'!$A$2:$A$346,0))</f>
         <v>East Ayrshire</v>
       </c>
       <c r="B19" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D19" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
-        <f t="array" ref="A20">INDEX('[1]Lookup Changes'!$C$2:$C$346,MATCH('[1]Short Name errors'!C20,'[1]Lookup Changes'!$A$2:$A$346,0))</f>
+        <f t="array" ref="A20">INDEX('[1]Lookup Changes'!$C$2:$C$346,MATCH('[1]Short Name errors'!C21,'[1]Lookup Changes'!$A$2:$A$346,0))</f>
         <v>East Ayrshire</v>
       </c>
       <c r="B20" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C20" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D20" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
-        <f t="array" ref="A21">INDEX('[1]Lookup Changes'!$C$2:$C$346,MATCH('[1]Short Name errors'!C21,'[1]Lookup Changes'!$A$2:$A$346,0))</f>
+        <f t="array" ref="A21">INDEX('[1]Lookup Changes'!$C$2:$C$346,MATCH('[1]Short Name errors'!C22,'[1]Lookup Changes'!$A$2:$A$346,0))</f>
         <v>East Ayrshire</v>
       </c>
       <c r="B21" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D21" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
-        <f t="array" ref="A22">INDEX('[1]Lookup Changes'!$C$2:$C$346,MATCH('[1]Short Name errors'!C22,'[1]Lookup Changes'!$A$2:$A$346,0))</f>
+        <f t="array" ref="A22">INDEX('[1]Lookup Changes'!$C$2:$C$346,MATCH('[1]Short Name errors'!C23,'[1]Lookup Changes'!$A$2:$A$346,0))</f>
         <v>East Ayrshire</v>
       </c>
       <c r="B22" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C22" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
-        <f t="array" ref="A23">INDEX('[1]Lookup Changes'!$C$2:$C$346,MATCH('[1]Short Name errors'!C23,'[1]Lookup Changes'!$A$2:$A$346,0))</f>
-        <v>East Ayrshire</v>
+        <f t="array" ref="A23">INDEX('[1]Lookup Changes'!$C$2:$C$346,MATCH('[1]Short Name errors'!C25,'[1]Lookup Changes'!$A$2:$A$346,0))</f>
+        <v>East Dunbartonshire</v>
       </c>
       <c r="B23" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C23" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D23" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
-        <f t="array" ref="A24">INDEX('[1]Lookup Changes'!$C$2:$C$346,MATCH('[1]Short Name errors'!C25,'[1]Lookup Changes'!$A$2:$A$346,0))</f>
+        <f t="array" ref="A24">INDEX('[1]Lookup Changes'!$C$2:$C$346,MATCH('[1]Short Name errors'!C26,'[1]Lookup Changes'!$A$2:$A$346,0))</f>
         <v>East Dunbartonshire</v>
       </c>
       <c r="B24" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C24" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
-        <f t="array" ref="A25">INDEX('[1]Lookup Changes'!$C$2:$C$346,MATCH('[1]Short Name errors'!C26,'[1]Lookup Changes'!$A$2:$A$346,0))</f>
+        <f t="array" ref="A25">INDEX('[1]Lookup Changes'!$C$2:$C$346,MATCH('[1]Short Name errors'!C27,'[1]Lookup Changes'!$A$2:$A$346,0))</f>
         <v>East Dunbartonshire</v>
       </c>
       <c r="B25" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C25" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D25" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
-        <f t="array" ref="A26">INDEX('[1]Lookup Changes'!$C$2:$C$346,MATCH('[1]Short Name errors'!C27,'[1]Lookup Changes'!$A$2:$A$346,0))</f>
+        <f t="array" ref="A26">INDEX('[1]Lookup Changes'!$C$2:$C$346,MATCH('[1]Short Name errors'!C28,'[1]Lookup Changes'!$A$2:$A$346,0))</f>
         <v>East Dunbartonshire</v>
       </c>
       <c r="B26" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C26" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D26" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
-        <f t="array" ref="A27">INDEX('[1]Lookup Changes'!$C$2:$C$346,MATCH('[1]Short Name errors'!C28,'[1]Lookup Changes'!$A$2:$A$346,0))</f>
+        <f t="array" ref="A27">INDEX('[1]Lookup Changes'!$C$2:$C$346,MATCH('[1]Short Name errors'!C29,'[1]Lookup Changes'!$A$2:$A$346,0))</f>
         <v>East Dunbartonshire</v>
       </c>
       <c r="B27" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C27" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D27" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
-        <f t="array" ref="A28">INDEX('[1]Lookup Changes'!$C$2:$C$346,MATCH('[1]Short Name errors'!C29,'[1]Lookup Changes'!$A$2:$A$346,0))</f>
+        <f t="array" ref="A28">INDEX('[1]Lookup Changes'!$C$2:$C$346,MATCH('[1]Short Name errors'!C30,'[1]Lookup Changes'!$A$2:$A$346,0))</f>
         <v>East Dunbartonshire</v>
       </c>
       <c r="B28" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C28" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D28" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
-        <f t="array" ref="A29">INDEX('[1]Lookup Changes'!$C$2:$C$346,MATCH('[1]Short Name errors'!C30,'[1]Lookup Changes'!$A$2:$A$346,0))</f>
+        <f t="array" ref="A29">INDEX('[1]Lookup Changes'!$C$2:$C$346,MATCH('[1]Short Name errors'!C31,'[1]Lookup Changes'!$A$2:$A$346,0))</f>
         <v>East Dunbartonshire</v>
       </c>
       <c r="B29" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C29" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D29" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="str">
-        <f t="array" ref="A30">INDEX('[1]Lookup Changes'!$C$2:$C$346,MATCH('[1]Short Name errors'!C31,'[1]Lookup Changes'!$A$2:$A$346,0))</f>
-        <v>East Dunbartonshire</v>
-      </c>
-      <c r="B30" t="s">
-        <v>293</v>
-      </c>
-      <c r="C30" t="s">
-        <v>83</v>
-      </c>
-      <c r="D30" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>